<commit_message>
adding 1 new excel and modified dashboard and .gitignore
</commit_message>
<xml_diff>
--- a/test-data/Identifiers.xlsx
+++ b/test-data/Identifiers.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Search Field</t>
   </si>
   <si>
     <t>//input[@name='q']</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>//div[@id='timeline']</t>
   </si>
 </sst>
 </file>
@@ -387,13 +393,13 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -405,8 +411,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
xpaths now will be handled from excel file
</commit_message>
<xml_diff>
--- a/test-data/Identifiers.xlsx
+++ b/test-data/Identifiers.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
+    <sheet name="loginpage" sheetId="2" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="1" r:id="rId2"/>
+    <sheet name="potusdashboard" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Search Field</t>
   </si>
@@ -26,6 +28,69 @@
   </si>
   <si>
     <t>//div[@id='timeline']</t>
+  </si>
+  <si>
+    <t>PageLoadElements</t>
+  </si>
+  <si>
+    <t>//div[@class='StaticLoggedOutHomePage-cell StaticLoggedOutHomePage-utilityBlock']</t>
+  </si>
+  <si>
+    <t>loginButton</t>
+  </si>
+  <si>
+    <t>//div[@class='StaticLoggedOutHomePage-buttons']/a[contains(text(),'Log in')]</t>
+  </si>
+  <si>
+    <t>userNameField</t>
+  </si>
+  <si>
+    <t>//input[@type='text' and @placeholder='Phone, email or username']</t>
+  </si>
+  <si>
+    <t>passwordField</t>
+  </si>
+  <si>
+    <t>//div[@class='clearfix field']/input[@name='session[password]']</t>
+  </si>
+  <si>
+    <t>loginButton2</t>
+  </si>
+  <si>
+    <t>//div[@class='clearfix']/button[text()='Log in']</t>
+  </si>
+  <si>
+    <t>//div[@class='ProfileNav']</t>
+  </si>
+  <si>
+    <t>followButton</t>
+  </si>
+  <si>
+    <t>(//span/button/span[text()='Follow'])[1]</t>
+  </si>
+  <si>
+    <t>followingButton</t>
+  </si>
+  <si>
+    <t>(//span/button/span[text()='Following'])[1]</t>
+  </si>
+  <si>
+    <t>logoutMenu</t>
+  </si>
+  <si>
+    <t>//a[@id='user-dropdown-toggle']</t>
+  </si>
+  <si>
+    <t>logoutbutton</t>
+  </si>
+  <si>
+    <t>//button[text()='Log out']</t>
+  </si>
+  <si>
+    <t>menuLoadWait</t>
+  </si>
+  <si>
+    <t>//div[@class='js-first-tabstop']/..</t>
   </si>
 </sst>
 </file>
@@ -41,7 +106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -51,6 +116,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -82,10 +153,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,9 +462,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -418,29 +565,84 @@
         <v>3</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>